<commit_message>
Updating plant survey datasheets
</commit_message>
<xml_diff>
--- a/Glacial_succession_survey/Plant_survey_DATA.xlsx
+++ b/Glacial_succession_survey/Plant_survey_DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ciaranorton/Documents/GitHub/Garibaldi/Glacial_succession_survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1C0BDA-D590-AA48-A378-71846FC3FB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00618CD9-86F9-E449-BBF7-8D439E2428EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19140" windowHeight="16420" firstSheet="4" activeTab="9" xr2:uid="{3D69C17B-FDC4-8D40-89DF-0D2A2855427F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" firstSheet="4" activeTab="11" xr2:uid="{3D69C17B-FDC4-8D40-89DF-0D2A2855427F}"/>
   </bookViews>
   <sheets>
     <sheet name="#1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4777" uniqueCount="660">
   <si>
     <t>Date:</t>
   </si>
@@ -1692,12 +1692,6 @@
     <t>GRAVEL</t>
   </si>
   <si>
-    <t>49 89738</t>
-  </si>
-  <si>
-    <t>122 98978</t>
-  </si>
-  <si>
     <t>WP31</t>
   </si>
   <si>
@@ -1722,9 +1716,6 @@
     <t>Orange mtn dandelion</t>
   </si>
   <si>
-    <t>ago</t>
-  </si>
-  <si>
     <t>Solidago</t>
   </si>
   <si>
@@ -1837,6 +1828,207 @@
   </si>
   <si>
     <t>3om</t>
+  </si>
+  <si>
+    <t>2, 0, 4, 4</t>
+  </si>
+  <si>
+    <t>2, 0, 0, 1</t>
+  </si>
+  <si>
+    <t>2, 3, 1, 2</t>
+  </si>
+  <si>
+    <t>1, 4, 3, 2</t>
+  </si>
+  <si>
+    <t>1, 3, 1, 3</t>
+  </si>
+  <si>
+    <t>0, 2, 4, 0</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 3</t>
+  </si>
+  <si>
+    <t>1, 1, 4, 2</t>
+  </si>
+  <si>
+    <t>wormskjoldii</t>
+  </si>
+  <si>
+    <t>Gramminoid</t>
+  </si>
+  <si>
+    <t>sp10</t>
+  </si>
+  <si>
+    <t>sp11</t>
+  </si>
+  <si>
+    <t>Edible thistle</t>
+  </si>
+  <si>
+    <t>Green spleenwort</t>
+  </si>
+  <si>
+    <t>Potentilla</t>
+  </si>
+  <si>
+    <t>glaucophyla</t>
+  </si>
+  <si>
+    <t>Fringed grass of parnasus</t>
+  </si>
+  <si>
+    <t>Ranunculus</t>
+  </si>
+  <si>
+    <t>eschscholtzii</t>
+  </si>
+  <si>
+    <t>Stelaria</t>
+  </si>
+  <si>
+    <t>32m</t>
+  </si>
+  <si>
+    <t>49° 89738</t>
+  </si>
+  <si>
+    <t>122° 98978</t>
+  </si>
+  <si>
+    <t>JG &amp; MS</t>
+  </si>
+  <si>
+    <t>49°91762</t>
+  </si>
+  <si>
+    <t>49°90371</t>
+  </si>
+  <si>
+    <t>122° 97991</t>
+  </si>
+  <si>
+    <t>122° 97969</t>
+  </si>
+  <si>
+    <t>CE05</t>
+  </si>
+  <si>
+    <t>CE02</t>
+  </si>
+  <si>
+    <t>1, 1, 1, 3</t>
+  </si>
+  <si>
+    <t>26m</t>
+  </si>
+  <si>
+    <t>2, 2, 2, 1</t>
+  </si>
+  <si>
+    <t>2.5m</t>
+  </si>
+  <si>
+    <t>dwarf hawksweed</t>
+  </si>
+  <si>
+    <t>Lewis monkeyflower</t>
+  </si>
+  <si>
+    <t>leptocarpum</t>
+  </si>
+  <si>
+    <t>arabidopsis</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>veronica</t>
+  </si>
+  <si>
+    <t>Grammminoid</t>
+  </si>
+  <si>
+    <t>spp3</t>
+  </si>
+  <si>
+    <t>spp4</t>
+  </si>
+  <si>
+    <t>4, 4, 1, 4</t>
+  </si>
+  <si>
+    <t>1, 0, 1, 4</t>
+  </si>
+  <si>
+    <t>1, 1, 0, 2</t>
+  </si>
+  <si>
+    <t>1, 0, 1, 0</t>
+  </si>
+  <si>
+    <t>spp7</t>
+  </si>
+  <si>
+    <t>escholtii</t>
+  </si>
+  <si>
+    <t>Orange mountain dandelion</t>
+  </si>
+  <si>
+    <t>Alpine ladyfern</t>
+  </si>
+  <si>
+    <t>Alpine sorrel</t>
+  </si>
+  <si>
+    <t>Oxyria</t>
+  </si>
+  <si>
+    <t>Dyrinia</t>
+  </si>
+  <si>
+    <t>Moss cameron</t>
+  </si>
+  <si>
+    <t>Cottonwood</t>
+  </si>
+  <si>
+    <t>Coltsfoot</t>
+  </si>
+  <si>
+    <t>Smooth alumroot</t>
+  </si>
+  <si>
+    <t>Flowering plant 1</t>
+  </si>
+  <si>
+    <t>3.5m</t>
+  </si>
+  <si>
+    <t>Shrubby cinguefoil</t>
+  </si>
+  <si>
+    <t>spp 9</t>
+  </si>
+  <si>
+    <t>spp 8</t>
+  </si>
+  <si>
+    <t>2, 2, 1, 3</t>
+  </si>
+  <si>
+    <t>2, 3, 1, 0</t>
+  </si>
+  <si>
+    <t>0, 0, 1, 4</t>
+  </si>
+  <si>
+    <t>Rolmie's Saxifrage</t>
   </si>
 </sst>
 </file>
@@ -4130,8 +4322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B921BFF-3F98-334E-BC5C-7564E0EE4CED}">
   <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView zoomScale="125" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5620,10 +5812,10 @@
       <c r="B72" s="16"/>
       <c r="C72" s="16"/>
       <c r="D72" s="17" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F72" s="16" t="s">
         <v>214</v>
@@ -5640,7 +5832,7 @@
         <v>132</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>226</v>
@@ -5657,7 +5849,7 @@
         <v>290</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="F74" s="16" t="s">
         <v>226</v>
@@ -5671,7 +5863,7 @@
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="19" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E75" s="19" t="s">
         <v>489</v>
@@ -5688,7 +5880,7 @@
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
       <c r="D76" s="17" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E76" s="17" t="s">
         <v>49</v>
@@ -5705,7 +5897,7 @@
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="19" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E77" s="19" t="s">
         <v>456</v>
@@ -5722,10 +5914,10 @@
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
       <c r="D78" s="19" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F78" s="16" t="s">
         <v>214</v>
@@ -5742,7 +5934,7 @@
         <v>349</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>214</v>
@@ -5756,10 +5948,10 @@
       <c r="B80" s="16"/>
       <c r="C80" s="16"/>
       <c r="D80" s="17" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="F80" s="16" t="s">
         <v>214</v>
@@ -5773,7 +5965,7 @@
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="19" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E81" s="19" t="s">
         <v>489</v>
@@ -5790,12 +5982,14 @@
       <c r="B82" s="16"/>
       <c r="C82" s="16"/>
       <c r="D82" s="17" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>572</v>
-      </c>
-      <c r="F82" s="16"/>
+        <v>569</v>
+      </c>
+      <c r="F82" s="16" t="s">
+        <v>593</v>
+      </c>
       <c r="G82" s="16"/>
       <c r="H82" s="16"/>
       <c r="I82" s="18"/>
@@ -5805,12 +5999,14 @@
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="19" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="F83" s="5"/>
+      <c r="F83" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="20"/>
@@ -5823,9 +6019,11 @@
         <v>349</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="F84" s="16"/>
+        <v>564</v>
+      </c>
+      <c r="F84" s="16" t="s">
+        <v>594</v>
+      </c>
       <c r="G84" s="16"/>
       <c r="H84" s="16"/>
       <c r="I84" s="18"/>
@@ -5835,12 +6033,14 @@
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="19" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="F85" s="5"/>
+        <v>565</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>425</v>
+      </c>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="20"/>
@@ -5853,9 +6053,11 @@
         <v>381</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>573</v>
-      </c>
-      <c r="F86" s="16"/>
+        <v>570</v>
+      </c>
+      <c r="F86" s="16" t="s">
+        <v>595</v>
+      </c>
       <c r="G86" s="16"/>
       <c r="H86" s="16"/>
       <c r="I86" s="18"/>
@@ -5865,12 +6067,14 @@
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="19" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>574</v>
-      </c>
-      <c r="F87" s="5"/>
+        <v>571</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>596</v>
+      </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
       <c r="I87" s="20"/>
@@ -5885,7 +6089,9 @@
       <c r="E88" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="F88" s="16"/>
+      <c r="F88" s="16" t="s">
+        <v>597</v>
+      </c>
       <c r="G88" s="16"/>
       <c r="H88" s="16"/>
       <c r="I88" s="18"/>
@@ -5898,9 +6104,11 @@
         <v>93</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>576</v>
-      </c>
-      <c r="F89" s="16"/>
+        <v>573</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>543</v>
+      </c>
       <c r="G89" s="16"/>
       <c r="H89" s="16"/>
       <c r="I89" s="18"/>
@@ -5910,12 +6118,14 @@
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="19" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E90" s="59" t="s">
-        <v>584</v>
-      </c>
-      <c r="F90" s="5"/>
+        <v>581</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>598</v>
+      </c>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="20"/>
@@ -5925,12 +6135,14 @@
       <c r="B91" s="16"/>
       <c r="C91" s="16"/>
       <c r="D91" s="17" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>559</v>
-      </c>
-      <c r="F91" s="16"/>
+        <v>556</v>
+      </c>
+      <c r="F91" s="16" t="s">
+        <v>282</v>
+      </c>
       <c r="G91" s="16"/>
       <c r="H91" s="16"/>
       <c r="I91" s="18"/>
@@ -5939,13 +6151,15 @@
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E92" s="19"/>
-      <c r="F92" s="5"/>
+      <c r="F92" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
       <c r="I92" s="20"/>
@@ -5954,13 +6168,15 @@
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
       <c r="C93" s="16" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E93" s="17"/>
-      <c r="F93" s="16"/>
+      <c r="F93" s="16" t="s">
+        <v>344</v>
+      </c>
       <c r="G93" s="16"/>
       <c r="H93" s="16"/>
       <c r="I93" s="18"/>
@@ -5970,12 +6186,14 @@
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="19" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E94" s="19" t="s">
-        <v>581</v>
-      </c>
-      <c r="F94" s="5"/>
+        <v>578</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
       <c r="I94" s="20"/>
@@ -5988,9 +6206,11 @@
         <v>347</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="F95" s="16"/>
+        <v>579</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>226</v>
+      </c>
       <c r="G95" s="16"/>
       <c r="H95" s="16"/>
       <c r="I95" s="18"/>
@@ -6005,7 +6225,9 @@
       <c r="E96" s="19" t="s">
         <v>528</v>
       </c>
-      <c r="F96" s="5"/>
+      <c r="F96" s="5" t="s">
+        <v>324</v>
+      </c>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
       <c r="I96" s="20"/>
@@ -6018,7 +6240,7 @@
         <v>125</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F97" s="16" t="s">
         <v>324</v>
@@ -6032,10 +6254,10 @@
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="19" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>314</v>
@@ -6049,7 +6271,7 @@
       <c r="B99" s="16"/>
       <c r="C99" s="16"/>
       <c r="D99" s="17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E99" s="17"/>
       <c r="F99" s="16" t="s">
@@ -6070,7 +6292,7 @@
         <v>489</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="G100" s="5"/>
       <c r="H100" s="5"/>
@@ -6081,10 +6303,10 @@
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
       <c r="D101" s="17" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="F101" s="16" t="s">
         <v>232</v>
@@ -6101,7 +6323,7 @@
         <v>176</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>232</v>
@@ -6115,10 +6337,10 @@
       <c r="B103" s="16"/>
       <c r="C103" s="16"/>
       <c r="D103" s="17" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E103" s="17" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F103" s="16" t="s">
         <v>232</v>
@@ -6246,8 +6468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AB9E82-BB6A-FA4A-B0CC-309E289AE3E9}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A60" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6321,7 +6543,7 @@
       <c r="D5" s="35"/>
       <c r="E5" s="43"/>
       <c r="F5" s="46" t="s">
-        <v>547</v>
+        <v>614</v>
       </c>
       <c r="G5" s="46"/>
       <c r="H5" s="45"/>
@@ -6336,7 +6558,7 @@
       <c r="D6" s="35"/>
       <c r="E6" s="43"/>
       <c r="F6" s="46" t="s">
-        <v>548</v>
+        <v>615</v>
       </c>
       <c r="G6" s="46"/>
       <c r="H6" s="45"/>
@@ -6387,7 +6609,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -7047,7 +7269,9 @@
       <c r="E40" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="20"/>
@@ -7111,7 +7335,7 @@
         <v>126</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
@@ -7199,7 +7423,7 @@
         <v>49</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
@@ -7245,7 +7469,7 @@
         <v>141</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
@@ -7312,7 +7536,7 @@
         <v>152</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
@@ -7442,7 +7666,7 @@
         <v>173</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
@@ -7465,7 +7689,7 @@
         <v>177</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
@@ -7534,7 +7758,9 @@
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="5"/>
+      <c r="F63" s="16" t="s">
+        <v>599</v>
+      </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="20"/>
@@ -7549,7 +7775,9 @@
         <v>297</v>
       </c>
       <c r="E64" s="17"/>
-      <c r="F64" s="16"/>
+      <c r="F64" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
       <c r="I64" s="18"/>
@@ -7560,9 +7788,13 @@
       <c r="C65" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="19"/>
+      <c r="D65" s="19" t="s">
+        <v>486</v>
+      </c>
       <c r="E65" s="19"/>
-      <c r="F65" s="5"/>
+      <c r="F65" s="16" t="s">
+        <v>600</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="20"/>
@@ -7571,13 +7803,15 @@
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>557</v>
+        <v>486</v>
       </c>
       <c r="E66" s="17"/>
-      <c r="F66" s="16"/>
+      <c r="F66" s="16" t="s">
+        <v>482</v>
+      </c>
       <c r="G66" s="16"/>
       <c r="H66" s="16"/>
       <c r="I66" s="18"/>
@@ -7586,9 +7820,15 @@
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="F67" s="5">
+        <v>1</v>
+      </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="20"/>
@@ -7596,10 +7836,16 @@
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="16"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="17"/>
+      <c r="C68" s="16" t="s">
+        <v>602</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>603</v>
+      </c>
       <c r="E68" s="17"/>
-      <c r="F68" s="16"/>
+      <c r="F68" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="G68" s="16"/>
       <c r="H68" s="16"/>
       <c r="I68" s="18"/>
@@ -7607,10 +7853,16 @@
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="19"/>
+      <c r="C69" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>604</v>
+      </c>
       <c r="E69" s="19"/>
-      <c r="F69" s="5"/>
+      <c r="F69" s="16" t="s">
+        <v>379</v>
+      </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="20"/>
@@ -7618,10 +7870,14 @@
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
       <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+      <c r="C70" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="D70" s="17"/>
       <c r="E70" s="17"/>
-      <c r="F70" s="16"/>
+      <c r="F70" s="16" t="s">
+        <v>215</v>
+      </c>
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
       <c r="I70" s="18"/>
@@ -7629,10 +7885,14 @@
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>433</v>
+      </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
-      <c r="F71" s="5"/>
+      <c r="F71" s="5" t="s">
+        <v>401</v>
+      </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="20"/>
@@ -7640,10 +7900,14 @@
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
       <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
+      <c r="C72" s="16" t="s">
+        <v>605</v>
+      </c>
       <c r="D72" s="17"/>
       <c r="E72" s="17"/>
-      <c r="F72" s="16"/>
+      <c r="F72" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="G72" s="16"/>
       <c r="H72" s="16"/>
       <c r="I72" s="18"/>
@@ -7651,10 +7915,14 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>606</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
-      <c r="F73" s="5"/>
+      <c r="F73" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="20"/>
@@ -7663,9 +7931,15 @@
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
       <c r="C74" s="16"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="16"/>
+      <c r="D74" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>216</v>
+      </c>
       <c r="G74" s="16"/>
       <c r="H74" s="16"/>
       <c r="I74" s="18"/>
@@ -7673,10 +7947,14 @@
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>609</v>
+      </c>
       <c r="D75" s="19"/>
       <c r="E75" s="19"/>
-      <c r="F75" s="5"/>
+      <c r="F75" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="20"/>
@@ -7685,9 +7963,15 @@
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="16"/>
+      <c r="D76" s="16" t="s">
+        <v>610</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>611</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>202</v>
+      </c>
       <c r="G76" s="16"/>
       <c r="H76" s="16"/>
       <c r="I76" s="18"/>
@@ -7696,9 +7980,13 @@
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
-      <c r="D77" s="19"/>
+      <c r="D77" s="19" t="s">
+        <v>612</v>
+      </c>
       <c r="E77" s="19"/>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>613</v>
+      </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="20"/>
@@ -7707,9 +7995,13 @@
       <c r="A78" s="16"/>
       <c r="B78" s="16"/>
       <c r="C78" s="16"/>
-      <c r="D78" s="17"/>
+      <c r="D78" s="17" t="s">
+        <v>487</v>
+      </c>
       <c r="E78" s="17"/>
-      <c r="F78" s="16"/>
+      <c r="F78" s="16" t="s">
+        <v>613</v>
+      </c>
       <c r="G78" s="16"/>
       <c r="H78" s="16"/>
       <c r="I78" s="18"/>
@@ -7718,9 +8010,13 @@
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
-      <c r="D79" s="19"/>
+      <c r="D79" s="19" t="s">
+        <v>391</v>
+      </c>
       <c r="E79" s="19"/>
-      <c r="F79" s="5"/>
+      <c r="F79" s="5" t="s">
+        <v>613</v>
+      </c>
       <c r="G79" s="5"/>
       <c r="H79" s="16"/>
       <c r="I79" s="20"/>
@@ -7809,10 +8105,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6895C5A-DE82-3942-B271-698B4D08AC34}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7825,7 +8121,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="34">
+        <v>45140</v>
+      </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -7838,7 +8136,9 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>616</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -7881,8 +8181,12 @@
       <c r="C5" s="8"/>
       <c r="D5" s="35"/>
       <c r="E5" s="43"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
+      <c r="F5" s="46" t="s">
+        <v>617</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>618</v>
+      </c>
       <c r="H5" s="45"/>
       <c r="I5" s="36"/>
     </row>
@@ -7894,8 +8198,12 @@
       <c r="C6" s="8"/>
       <c r="D6" s="35"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
+      <c r="F6" s="46" t="s">
+        <v>620</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>619</v>
+      </c>
       <c r="H6" s="45"/>
       <c r="I6" s="36"/>
     </row>
@@ -7941,8 +8249,12 @@
       <c r="E9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>622</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
@@ -7962,7 +8274,9 @@
       <c r="E10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>304</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="18"/>
@@ -8025,7 +8339,9 @@
       <c r="E13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="20"/>
@@ -8172,7 +8488,9 @@
       <c r="E20" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="16"/>
+      <c r="F20" s="16" t="s">
+        <v>196</v>
+      </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16"/>
       <c r="I20" s="18"/>
@@ -8193,7 +8511,9 @@
       <c r="E21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="20"/>
@@ -8298,7 +8618,9 @@
       <c r="E26" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="5" t="s">
+        <v>222</v>
+      </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="20"/>
@@ -8382,7 +8704,9 @@
       <c r="E30" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>236</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="20"/>
@@ -8592,7 +8916,9 @@
       <c r="E40" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="5" t="s">
+        <v>623</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="20"/>
@@ -8655,7 +8981,9 @@
       <c r="E43" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="24"/>
+      <c r="F43" s="24" t="s">
+        <v>624</v>
+      </c>
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
       <c r="I43" s="26"/>
@@ -8718,7 +9046,9 @@
       <c r="E46" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="F46" s="16"/>
+      <c r="F46" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="G46" s="16"/>
       <c r="H46" s="16"/>
       <c r="I46" s="18"/>
@@ -8781,7 +9111,9 @@
       <c r="E49" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="F49" s="5"/>
+      <c r="F49" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
       <c r="I49" s="20"/>
@@ -8802,7 +9134,9 @@
       <c r="E50" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="F50" s="16"/>
+      <c r="F50" s="16" t="s">
+        <v>282</v>
+      </c>
       <c r="G50" s="16"/>
       <c r="H50" s="16"/>
       <c r="I50" s="18"/>
@@ -8823,7 +9157,9 @@
       <c r="E51" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="F51" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="20"/>
@@ -8844,7 +9180,9 @@
       <c r="E52" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="F52" s="16"/>
+      <c r="F52" s="16" t="s">
+        <v>245</v>
+      </c>
       <c r="G52" s="16"/>
       <c r="H52" s="16"/>
       <c r="I52" s="18"/>
@@ -8886,7 +9224,9 @@
       <c r="E54" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="F54" s="16"/>
+      <c r="F54" s="16" t="s">
+        <v>625</v>
+      </c>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="18"/>
@@ -8949,7 +9289,9 @@
       <c r="E57" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="F57" s="5"/>
+      <c r="F57" s="5" t="s">
+        <v>626</v>
+      </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="20"/>
@@ -8991,8 +9333,12 @@
       <c r="E59" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="F59" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>511</v>
+      </c>
       <c r="H59" s="5"/>
       <c r="I59" s="20"/>
     </row>
@@ -9054,10 +9400,14 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>627</v>
+      </c>
       <c r="D63" s="19"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="5"/>
+      <c r="F63" s="5" t="s">
+        <v>378</v>
+      </c>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
       <c r="I63" s="20"/>
@@ -9065,10 +9415,14 @@
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
+      <c r="C64" s="16" t="s">
+        <v>628</v>
+      </c>
       <c r="D64" s="17"/>
       <c r="E64" s="17"/>
-      <c r="F64" s="16"/>
+      <c r="F64" s="16" t="s">
+        <v>639</v>
+      </c>
       <c r="G64" s="16"/>
       <c r="H64" s="16"/>
       <c r="I64" s="18"/>
@@ -9076,10 +9430,15 @@
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="5"/>
+      <c r="D65" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>496</v>
+      </c>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
       <c r="I65" s="20"/>
@@ -9087,10 +9446,18 @@
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="16"/>
+      <c r="C66" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>638</v>
+      </c>
       <c r="G66" s="16"/>
       <c r="H66" s="16"/>
       <c r="I66" s="18"/>
@@ -9099,42 +9466,68 @@
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="5"/>
+      <c r="D67" s="19" t="s">
+        <v>632</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="F67" s="16" t="s">
+        <v>637</v>
+      </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="20"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" s="16"/>
+      <c r="A68" s="16" t="s">
+        <v>633</v>
+      </c>
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
       <c r="D68" s="17"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
+      <c r="E68" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="H68" s="16"/>
       <c r="I68" s="18"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="5"/>
+      <c r="A69" s="5" t="s">
+        <v>633</v>
+      </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="5"/>
+      <c r="E69" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
       <c r="I69" s="20"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="16"/>
+      <c r="A70" s="16" t="s">
+        <v>633</v>
+      </c>
       <c r="B70" s="16"/>
       <c r="C70" s="16"/>
       <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="16"/>
+      <c r="E70" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="F70" s="16" t="s">
+        <v>631</v>
+      </c>
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
       <c r="I70" s="18"/>
@@ -9142,10 +9535,14 @@
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>433</v>
+      </c>
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
-      <c r="F71" s="5"/>
+      <c r="F71" s="16" t="s">
+        <v>262</v>
+      </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
       <c r="I71" s="20"/>
@@ -9154,9 +9551,15 @@
       <c r="A72" s="16"/>
       <c r="B72" s="16"/>
       <c r="C72" s="16"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="16"/>
+      <c r="D72" s="17" t="s">
+        <v>610</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>641</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="G72" s="16"/>
       <c r="H72" s="16"/>
       <c r="I72" s="18"/>
@@ -9164,10 +9567,14 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>642</v>
+      </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
-      <c r="F73" s="5"/>
+      <c r="F73" s="16" t="s">
+        <v>652</v>
+      </c>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
       <c r="I73" s="20"/>
@@ -9175,10 +9582,14 @@
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="16"/>
       <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
+      <c r="C74" s="16" t="s">
+        <v>643</v>
+      </c>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="G74" s="16"/>
       <c r="H74" s="16"/>
       <c r="I74" s="18"/>
@@ -9186,10 +9597,16 @@
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="5"/>
+      <c r="E75" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>220</v>
+      </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
       <c r="I75" s="20"/>
@@ -9197,10 +9614,18 @@
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="17"/>
-      <c r="F76" s="16"/>
+      <c r="C76" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>645</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>646</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>230</v>
+      </c>
       <c r="G76" s="16"/>
       <c r="H76" s="16"/>
       <c r="I76" s="18"/>
@@ -9208,10 +9633,14 @@
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
+      <c r="C77" s="5" t="s">
+        <v>647</v>
+      </c>
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>229</v>
+      </c>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="20"/>
@@ -9219,10 +9648,16 @@
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
+      <c r="C78" s="16" t="s">
+        <v>452</v>
+      </c>
       <c r="D78" s="17"/>
-      <c r="E78" s="17"/>
-      <c r="F78" s="16"/>
+      <c r="E78" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="F78" s="16" t="s">
+        <v>230</v>
+      </c>
       <c r="G78" s="16"/>
       <c r="H78" s="16"/>
       <c r="I78" s="18"/>
@@ -9230,10 +9665,14 @@
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
+      <c r="C79" s="5" t="s">
+        <v>648</v>
+      </c>
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
-      <c r="F79" s="5"/>
+      <c r="F79" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="G79" s="5"/>
       <c r="H79" s="16"/>
       <c r="I79" s="20"/>
@@ -9241,10 +9680,14 @@
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
+      <c r="C80" s="16" t="s">
+        <v>649</v>
+      </c>
       <c r="D80" s="17"/>
       <c r="E80" s="17"/>
-      <c r="F80" s="16"/>
+      <c r="F80" s="16" t="s">
+        <v>502</v>
+      </c>
       <c r="G80" s="16"/>
       <c r="H80" s="47"/>
       <c r="I80" s="18"/>
@@ -9252,10 +9695,14 @@
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
+      <c r="C81" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="D81" s="19"/>
       <c r="E81" s="19"/>
-      <c r="F81" s="5"/>
+      <c r="F81" s="5" t="s">
+        <v>276</v>
+      </c>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
       <c r="I81" s="20"/>
@@ -9263,10 +9710,14 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
+      <c r="C82" s="16" t="s">
+        <v>650</v>
+      </c>
       <c r="D82" s="17"/>
       <c r="E82" s="17"/>
-      <c r="F82" s="16"/>
+      <c r="F82" s="16" t="s">
+        <v>214</v>
+      </c>
       <c r="G82" s="16"/>
       <c r="H82" s="16"/>
       <c r="I82" s="18"/>
@@ -9274,10 +9725,14 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>651</v>
+      </c>
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
-      <c r="F83" s="5"/>
+      <c r="F83" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
       <c r="I83" s="20"/>
@@ -9285,35 +9740,143 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
+      <c r="C84" s="16" t="s">
+        <v>653</v>
+      </c>
       <c r="D84" s="17"/>
       <c r="E84" s="17"/>
       <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
+      <c r="G84" s="16" t="s">
+        <v>656</v>
+      </c>
       <c r="H84" s="16"/>
       <c r="I84" s="18"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" s="5"/>
+      <c r="A85" s="5" t="s">
+        <v>602</v>
+      </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
+      <c r="E85" s="19" t="s">
+        <v>655</v>
+      </c>
       <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
+      <c r="G85" s="5" t="s">
+        <v>657</v>
+      </c>
       <c r="H85" s="5"/>
       <c r="I85" s="20"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" s="16"/>
+      <c r="A86" s="16" t="s">
+        <v>602</v>
+      </c>
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
       <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
+      <c r="E86" s="17" t="s">
+        <v>654</v>
+      </c>
       <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
+      <c r="G86" s="16" t="s">
+        <v>658</v>
+      </c>
       <c r="H86" s="16"/>
       <c r="I86" s="18"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H87" s="5"/>
+      <c r="I87" s="20"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="16"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="17"/>
+      <c r="E88" s="17"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+      <c r="I89" s="20"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="17"/>
+      <c r="E90" s="17"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="18"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="20"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="17"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="20"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" s="16"/>
+      <c r="B94" s="16"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>